<commit_message>
Adding new indicators proposal
</commit_message>
<xml_diff>
--- a/Data/new_indicators.xlsx
+++ b/Data/new_indicators.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/tbenschop_worldbank_org/Documents/Documents/GitHub/WDI_GHG_emissions/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE174A3D-8A03-460F-8B41-FA1EC7767F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{CE174A3D-8A03-460F-8B41-FA1EC7767F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{185E3363-3B6E-4BB5-9CBE-4C53426A2D48}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3FA54C67-01C4-4850-B257-DA34E1F0B588}"/>
   </bookViews>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="75">
-  <si>
-    <t>Variable Code</t>
-  </si>
-  <si>
-    <t>Variable Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="124">
   <si>
     <t>Gases</t>
   </si>
@@ -259,13 +253,166 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2E.PC</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Carbon Dioxide (CO2) (Total excluding LULUCF) per capita</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: All Kyoto Gases (Total excluding LULUCF) per capita</t>
+  </si>
+  <si>
+    <t>EN.GHG.TOTL.PC</t>
+  </si>
+  <si>
+    <t>TOTL</t>
+  </si>
+  <si>
+    <t>CO2E</t>
+  </si>
+  <si>
+    <t>METH</t>
+  </si>
+  <si>
+    <t>NOXE</t>
+  </si>
+  <si>
+    <t>FGAS</t>
+  </si>
+  <si>
+    <t>Sector_code</t>
+  </si>
+  <si>
+    <t>Gas_code</t>
+  </si>
+  <si>
+    <t>Indicator Name</t>
+  </si>
+  <si>
+    <t>Indicator Code</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>absolute emissions</t>
+  </si>
+  <si>
+    <t>Land Use, Land Use Change, and Forestry</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Carbon Dioxide (CO2) (Sector = LULUCF)</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Methane (CH4) (Sector = LULUCF)</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Nitrous Oxide (N2O) (Sector = LULUCF)</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>per capita</t>
+  </si>
+  <si>
+    <t>per GDP</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: All Kyoto Gases (Total excluding LULUCF) per 2017 PPP $ of GDP</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Carbon Dioxide (CO2) (Total excluding LULUCF) per 2017 PPP $ of GDP</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Carbon Dioxide (CO2) (Total excluding LULUCF) per 2017 US $ of GDP</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: All Kyoto Gases (Total excluding LULUCF) per 2017 US$ of GDP</t>
+  </si>
+  <si>
+    <t>% change</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: All Kyoto Gases (Total excluding LULUCF) % change from 1990</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Carbon Dioxide (CO2) (Total excluding LULUCF) % change from 1990</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Methane (CH4) (Total excluding LULUCF) % change from 1990</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Nitrous Oxide (N2O) (Total excluding LULUCF) % change from 1990</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Carbon Dioxide (CO2) (Total excluding LULUCF) share of total GHG emissions</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Methane (CH4) (Total excluding LULUCF) share of total GHG emissions</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Nitrous Oxide (N2O) (Total excluding LULUCF) share of total GHG emissions</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions: Fluorinated Gases (Total excluding LULUCF) share of total GHG emissions</t>
+  </si>
+  <si>
+    <t>share of total</t>
+  </si>
+  <si>
+    <t>EN.GHG.TOTL.PP.GD</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2E.PP.GD</t>
+  </si>
+  <si>
+    <t>EN.GHG.TOTL.KD.GD</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2E.KD.GD</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2E.LU.KT.CE</t>
+  </si>
+  <si>
+    <t>EN.GHG.METH.LU.KT.CE</t>
+  </si>
+  <si>
+    <t>EN.GHG.NOXE.LU.KT.CE</t>
+  </si>
+  <si>
+    <t>EN.GHG.TOTL.ZG</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2E.ZG</t>
+  </si>
+  <si>
+    <t>EN.GHG.METH.ZG</t>
+  </si>
+  <si>
+    <t>EN.GHG.N2OX.ZG</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2E.ZS</t>
+  </si>
+  <si>
+    <t>EN.GHG.METH.ZS</t>
+  </si>
+  <si>
+    <t>EN.GHG.N2OX.ZS</t>
+  </si>
+  <si>
+    <t>EN.GHG.FGAS.ZS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +426,34 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -302,12 +477,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,632 +802,1253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A50484-D318-4EBD-AF4F-027A57CD92DB}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="C32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="B33" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>